<commit_message>
[update] update simulation python
</commit_message>
<xml_diff>
--- a/simulation/python/Book1 copy 4.xlsx
+++ b/simulation/python/Book1 copy 4.xlsx
@@ -120,17 +120,17 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="B1" s="0" t="n">
-        <v>210</v>
+        <v>40</v>
       </c>
       <c r="C1" s="0" t="n">
         <v>300</v>
@@ -164,7 +164,7 @@
         <v>240</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>225</v>
+        <v>185</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>25</v>
@@ -190,7 +190,7 @@
         <v>25</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>